<commit_message>
Erdungskontrolle kiegészítések és custom sorok
</commit_message>
<xml_diff>
--- a/public/templates/Abnahme FRAGEN.xlsx
+++ b/public/templates/Abnahme FRAGEN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\APROD\Aprod\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD404F5-36E1-4B30-94C0-3842BEC03543}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F290871-1691-4C76-B345-D40882DE8F0D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="41280" windowHeight="13260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1338,7 +1338,7 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1349,6 +1349,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFE6E6FA"/>
         <bgColor rgb="FFE6E6FA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1435,7 +1447,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1456,6 +1468,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -1739,7 +1755,7 @@
   <dimension ref="A1:Y49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1883,315 +1899,315 @@
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
     </row>
-    <row r="3" spans="1:25" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A3" s="1">
+    <row r="3" spans="1:25" s="15" customFormat="1" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A3" s="14">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1" t="s">
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="M3" s="1">
+      <c r="M3" s="14">
         <v>2</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="N3" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O3" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1" t="s">
+      <c r="R3" s="14"/>
+      <c r="S3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-    </row>
-    <row r="4" spans="1:25" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A4" s="1">
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14"/>
+      <c r="W3" s="14"/>
+      <c r="X3" s="14"/>
+      <c r="Y3" s="14"/>
+    </row>
+    <row r="4" spans="1:25" s="17" customFormat="1" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A4" s="16">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1" t="s">
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="M4" s="1">
+      <c r="M4" s="16">
         <v>3</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="N4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="O4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="P4" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="Q4" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1" t="s">
+      <c r="R4" s="16"/>
+      <c r="S4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-    </row>
-    <row r="5" spans="1:25" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A5" s="1">
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="16"/>
+    </row>
+    <row r="5" spans="1:25" s="17" customFormat="1" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A5" s="16">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1" t="s">
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="M5" s="1">
+      <c r="M5" s="16">
         <v>4</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N5" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="P5" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="Q5" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1" t="s">
+      <c r="R5" s="16"/>
+      <c r="S5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-    </row>
-    <row r="6" spans="1:25" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A6" s="1">
+      <c r="T5" s="16"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="16"/>
+      <c r="W5" s="16"/>
+      <c r="X5" s="16"/>
+      <c r="Y5" s="16"/>
+    </row>
+    <row r="6" spans="1:25" s="17" customFormat="1" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A6" s="16">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1" t="s">
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="M6" s="1">
+      <c r="M6" s="16">
         <v>5</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="N6" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="O6" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="P6" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="Q6" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1" t="s">
+      <c r="R6" s="16"/>
+      <c r="S6" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1" t="s">
+      <c r="T6" s="16"/>
+      <c r="U6" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-    </row>
-    <row r="7" spans="1:25" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A7" s="1">
+      <c r="V6" s="16"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="16"/>
+      <c r="Y6" s="16"/>
+    </row>
+    <row r="7" spans="1:25" s="17" customFormat="1" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A7" s="16">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1" t="s">
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="M7" s="1">
+      <c r="M7" s="16">
         <v>6</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="N7" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="O7" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="P7" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="Q7" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1" t="s">
+      <c r="R7" s="16"/>
+      <c r="S7" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1" t="s">
+      <c r="T7" s="16"/>
+      <c r="U7" s="16" t="s">
         <v>402</v>
       </c>
-      <c r="V7" s="1"/>
-      <c r="W7" s="1"/>
-      <c r="X7" s="1"/>
-      <c r="Y7" s="1"/>
-    </row>
-    <row r="8" spans="1:25" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A8" s="1">
+      <c r="V7" s="16"/>
+      <c r="W7" s="16"/>
+      <c r="X7" s="16"/>
+      <c r="Y7" s="16"/>
+    </row>
+    <row r="8" spans="1:25" s="15" customFormat="1" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A8" s="14">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1" t="s">
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="M8" s="1">
+      <c r="M8" s="14">
         <v>7</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="N8" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="O8" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="P8" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="Q8" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1" t="s">
+      <c r="R8" s="14"/>
+      <c r="S8" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="T8" s="1"/>
-      <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
-      <c r="W8" s="1"/>
-      <c r="X8" s="1"/>
-      <c r="Y8" s="1"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="14"/>
+      <c r="V8" s="14"/>
+      <c r="W8" s="14"/>
+      <c r="X8" s="14"/>
+      <c r="Y8" s="14"/>
     </row>
     <row r="9" spans="1:25" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A9" s="1">
@@ -2244,58 +2260,58 @@
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
     </row>
-    <row r="10" spans="1:25" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A10" s="1">
+    <row r="10" spans="1:25" s="15" customFormat="1" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A10" s="14">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1" t="s">
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="M10" s="1">
+      <c r="M10" s="14">
         <v>9</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="N10" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="O10" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="P10" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="Q10" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1" t="s">
+      <c r="R10" s="14"/>
+      <c r="S10" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1" t="s">
+      <c r="T10" s="14"/>
+      <c r="U10" s="14" t="s">
         <v>403</v>
       </c>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
+      <c r="V10" s="14"/>
+      <c r="W10" s="14"/>
+      <c r="X10" s="14"/>
+      <c r="Y10" s="14"/>
     </row>
     <row r="11" spans="1:25" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A11" s="1">
@@ -5398,7 +5414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D002D2D2-CD20-48F6-B52A-09E6DFF1BA72}">
   <dimension ref="A1:Q69"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
User delete / Login / Password reset
</commit_message>
<xml_diff>
--- a/public/templates/Abnahme FRAGEN.xlsx
+++ b/public/templates/Abnahme FRAGEN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\APROD\Aprod\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F290871-1691-4C76-B345-D40882DE8F0D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD404F5-36E1-4B30-94C0-3842BEC03543}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="41280" windowHeight="13260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1338,7 +1338,7 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1349,18 +1349,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFE6E6FA"/>
         <bgColor rgb="FFE6E6FA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1447,7 +1435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1468,10 +1456,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -1755,7 +1739,7 @@
   <dimension ref="A1:Y49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1899,315 +1883,315 @@
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
     </row>
-    <row r="3" spans="1:25" s="15" customFormat="1" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A3" s="14">
+    <row r="3" spans="1:25" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14" t="s">
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M3" s="14">
+      <c r="M3" s="1">
         <v>2</v>
       </c>
-      <c r="N3" s="14" t="s">
+      <c r="N3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O3" s="14" t="s">
+      <c r="O3" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="P3" s="14" t="s">
+      <c r="P3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Q3" s="14" t="s">
+      <c r="Q3" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14" t="s">
+      <c r="R3" s="1"/>
+      <c r="S3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14"/>
-      <c r="V3" s="14"/>
-      <c r="W3" s="14"/>
-      <c r="X3" s="14"/>
-      <c r="Y3" s="14"/>
-    </row>
-    <row r="4" spans="1:25" s="17" customFormat="1" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A4" s="16">
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+    </row>
+    <row r="4" spans="1:25" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16" t="s">
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M4" s="16">
+      <c r="M4" s="1">
         <v>3</v>
       </c>
-      <c r="N4" s="16" t="s">
+      <c r="N4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O4" s="16" t="s">
+      <c r="O4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P4" s="16" t="s">
+      <c r="P4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Q4" s="16" t="s">
+      <c r="Q4" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16" t="s">
+      <c r="R4" s="1"/>
+      <c r="S4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="T4" s="16"/>
-      <c r="U4" s="16"/>
-      <c r="V4" s="16"/>
-      <c r="W4" s="16"/>
-      <c r="X4" s="16"/>
-      <c r="Y4" s="16"/>
-    </row>
-    <row r="5" spans="1:25" s="17" customFormat="1" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A5" s="16">
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+    </row>
+    <row r="5" spans="1:25" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16" t="s">
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M5" s="16">
+      <c r="M5" s="1">
         <v>4</v>
       </c>
-      <c r="N5" s="16" t="s">
+      <c r="N5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O5" s="16" t="s">
+      <c r="O5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P5" s="16" t="s">
+      <c r="P5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Q5" s="16" t="s">
+      <c r="Q5" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="R5" s="16"/>
-      <c r="S5" s="16" t="s">
+      <c r="R5" s="1"/>
+      <c r="S5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="T5" s="16"/>
-      <c r="U5" s="16"/>
-      <c r="V5" s="16"/>
-      <c r="W5" s="16"/>
-      <c r="X5" s="16"/>
-      <c r="Y5" s="16"/>
-    </row>
-    <row r="6" spans="1:25" s="17" customFormat="1" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A6" s="16">
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+    </row>
+    <row r="6" spans="1:25" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16" t="s">
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M6" s="16">
+      <c r="M6" s="1">
         <v>5</v>
       </c>
-      <c r="N6" s="16" t="s">
+      <c r="N6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O6" s="16" t="s">
+      <c r="O6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="P6" s="16" t="s">
+      <c r="P6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Q6" s="16" t="s">
+      <c r="Q6" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="R6" s="16"/>
-      <c r="S6" s="16" t="s">
+      <c r="R6" s="1"/>
+      <c r="S6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T6" s="16"/>
-      <c r="U6" s="16" t="s">
+      <c r="T6" s="1"/>
+      <c r="U6" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="V6" s="16"/>
-      <c r="W6" s="16"/>
-      <c r="X6" s="16"/>
-      <c r="Y6" s="16"/>
-    </row>
-    <row r="7" spans="1:25" s="17" customFormat="1" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A7" s="16">
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+    </row>
+    <row r="7" spans="1:25" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16" t="s">
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M7" s="16">
+      <c r="M7" s="1">
         <v>6</v>
       </c>
-      <c r="N7" s="16" t="s">
+      <c r="N7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O7" s="16" t="s">
+      <c r="O7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="P7" s="16" t="s">
+      <c r="P7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Q7" s="16" t="s">
+      <c r="Q7" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="R7" s="16"/>
-      <c r="S7" s="16" t="s">
+      <c r="R7" s="1"/>
+      <c r="S7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T7" s="16"/>
-      <c r="U7" s="16" t="s">
+      <c r="T7" s="1"/>
+      <c r="U7" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="V7" s="16"/>
-      <c r="W7" s="16"/>
-      <c r="X7" s="16"/>
-      <c r="Y7" s="16"/>
-    </row>
-    <row r="8" spans="1:25" s="15" customFormat="1" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A8" s="14">
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+    </row>
+    <row r="8" spans="1:25" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14" t="s">
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M8" s="14">
+      <c r="M8" s="1">
         <v>7</v>
       </c>
-      <c r="N8" s="14" t="s">
+      <c r="N8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O8" s="14" t="s">
+      <c r="O8" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="P8" s="14" t="s">
+      <c r="P8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Q8" s="14" t="s">
+      <c r="Q8" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14" t="s">
+      <c r="R8" s="1"/>
+      <c r="S8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T8" s="14"/>
-      <c r="U8" s="14"/>
-      <c r="V8" s="14"/>
-      <c r="W8" s="14"/>
-      <c r="X8" s="14"/>
-      <c r="Y8" s="14"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
     </row>
     <row r="9" spans="1:25" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A9" s="1">
@@ -2260,58 +2244,58 @@
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
     </row>
-    <row r="10" spans="1:25" s="15" customFormat="1" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A10" s="14">
+    <row r="10" spans="1:25" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14" t="s">
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M10" s="14">
+      <c r="M10" s="1">
         <v>9</v>
       </c>
-      <c r="N10" s="14" t="s">
+      <c r="N10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O10" s="14" t="s">
+      <c r="O10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P10" s="14" t="s">
+      <c r="P10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Q10" s="14" t="s">
+      <c r="Q10" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="R10" s="14"/>
-      <c r="S10" s="14" t="s">
+      <c r="R10" s="1"/>
+      <c r="S10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="T10" s="14"/>
-      <c r="U10" s="14" t="s">
+      <c r="T10" s="1"/>
+      <c r="U10" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="V10" s="14"/>
-      <c r="W10" s="14"/>
-      <c r="X10" s="14"/>
-      <c r="Y10" s="14"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
     </row>
     <row r="11" spans="1:25" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A11" s="1">
@@ -5414,7 +5398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D002D2D2-CD20-48F6-B52A-09E6DFF1BA72}">
   <dimension ref="A1:Q69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Kérdések vastag keret javítás
</commit_message>
<xml_diff>
--- a/public/templates/Abnahme FRAGEN.xlsx
+++ b/public/templates/Abnahme FRAGEN.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\APROD\Aprod\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PWA\Aprod\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD404F5-36E1-4B30-94C0-3842BEC03543}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03FDE3B-8D95-40EC-93D4-85390CE32F49}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="41280" windowHeight="13260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20448" windowHeight="9468" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="questions" sheetId="2" r:id="rId1"/>
@@ -1738,8 +1738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C829CC3F-6FE0-4C51-9144-6919D0578DEB}">
   <dimension ref="A1:Y49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2238,7 +2238,9 @@
         <v>29</v>
       </c>
       <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
+      <c r="U9" s="1" t="s">
+        <v>403</v>
+      </c>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
@@ -2289,9 +2291,7 @@
         <v>31</v>
       </c>
       <c r="T10" s="1"/>
-      <c r="U10" s="1" t="s">
-        <v>403</v>
-      </c>
+      <c r="U10" s="1"/>
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>

</xml_diff>

<commit_message>
Nem tom mi de biztos jó
</commit_message>
<xml_diff>
--- a/public/templates/Abnahme FRAGEN.xlsx
+++ b/public/templates/Abnahme FRAGEN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PWA\Aprod\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43922B6-B770-4DA5-9EEA-DB0D7A5134A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDA0670-A670-438B-B3D2-7E935F26467E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20448" windowHeight="9468" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1771,8 +1771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C829CC3F-6FE0-4C51-9144-6919D0578DEB}">
   <dimension ref="A1:Z49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H13" workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+    <sheetView tabSelected="1" topLeftCell="F13" workbookViewId="0">
+      <selection activeCell="F17" sqref="A17:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>